<commit_message>
save no licenzion files
</commit_message>
<xml_diff>
--- a/platform_scrapper/CANNABIS_RESULTS/found_IDs.xlsx
+++ b/platform_scrapper/CANNABIS_RESULTS/found_IDs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9366" uniqueCount="3789">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9700" uniqueCount="3923">
   <si>
     <t>BURLINGTON</t>
   </si>
@@ -11383,6 +11383,408 @@
   </si>
   <si>
     <t>628-630 BLOOR ST</t>
+  </si>
+  <si>
+    <t>https://www.smokelab.ca/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2021/05/27</t>
+  </si>
+  <si>
+    <t>1234 KING ST W</t>
+  </si>
+  <si>
+    <t>Smoke Lab Cannabis - King West</t>
+  </si>
+  <si>
+    <t>http://www.spot420.ca/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2023/11/17</t>
+  </si>
+  <si>
+    <t>2180 CREDIT VALLEY RD UNIT 102</t>
+  </si>
+  <si>
+    <t>Spot420 The Cannabis Store</t>
+  </si>
+  <si>
+    <t>http://www.stickynuggzinc.com/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2023/03/04</t>
+  </si>
+  <si>
+    <t>85 COTTRELLE BLVD UNIT 3</t>
+  </si>
+  <si>
+    <t>Sticky Nuggz Cottrelle Inc.</t>
+  </si>
+  <si>
+    <t>https://stickynuggzinc.ca/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2022/04/11</t>
+  </si>
+  <si>
+    <t>354 WELLINGTON ST UNIT B</t>
+  </si>
+  <si>
+    <t>Sticky Nuggz London Wellington Inc.</t>
+  </si>
+  <si>
+    <t>https://superetteshop.com/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2021/07/02</t>
+  </si>
+  <si>
+    <t>2 OSSINGTON AVE UNIT 1</t>
+  </si>
+  <si>
+    <t>http://southernleafhemp.co/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2020/10/16</t>
+  </si>
+  <si>
+    <t>5236 HIGHWAY 12 SOUTH, UNIT B</t>
+  </si>
+  <si>
+    <t>SUPREME LEAF CANNABIS COMPANY</t>
+  </si>
+  <si>
+    <t>RAMARA</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2021/06/19</t>
+  </si>
+  <si>
+    <t>4651 SHEPPARD AVE E UNIT S102</t>
+  </si>
+  <si>
+    <t>Tampi Incorporation</t>
+  </si>
+  <si>
+    <t>https://www.tbcontario.com/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2021/11/19</t>
+  </si>
+  <si>
+    <t>45 STANLEY ST UNIT 200</t>
+  </si>
+  <si>
+    <t>https://thccanada.ca/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2023/02/02</t>
+  </si>
+  <si>
+    <t>38 BLUE JAYS WAY UNIT 5</t>
+  </si>
+  <si>
+    <t>THC CANADA</t>
+  </si>
+  <si>
+    <t>10 BRIDGEPORT RD W</t>
+  </si>
+  <si>
+    <t>The Cannabist Shop - Bridgeport W</t>
+  </si>
+  <si>
+    <t>https://www.cannabistshop.ca/london-dispensary</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2021/08/28</t>
+  </si>
+  <si>
+    <t>62 WHARNCLIFFE RD N</t>
+  </si>
+  <si>
+    <t>THE CANNABIST SHOP - WHARNCLIFFE</t>
+  </si>
+  <si>
+    <t>250 ALBERT ST SUITE 107</t>
+  </si>
+  <si>
+    <t>The Green Closet Waterloo</t>
+  </si>
+  <si>
+    <t>https://www.thegreenroomcannabis.ca/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2021/09/11</t>
+  </si>
+  <si>
+    <t>109 KING ST W</t>
+  </si>
+  <si>
+    <t>The Green Room - King W</t>
+  </si>
+  <si>
+    <t>https://cbd.puffingbird.com/ontario/guelph/the-green-room</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2021/08/13</t>
+  </si>
+  <si>
+    <t>89 MACDONELL ST</t>
+  </si>
+  <si>
+    <t>The Green Room - Macdonell</t>
+  </si>
+  <si>
+    <t>https://thehunnypot.com/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2021/10/14</t>
+  </si>
+  <si>
+    <t>3010 COLONEL TALBOT RD SUITE 1</t>
+  </si>
+  <si>
+    <t>['No delivery / Temporarily closed']</t>
+  </si>
+  <si>
+    <t>http://thenugco.ca/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2022/02/24</t>
+  </si>
+  <si>
+    <t>514 RITSON RD S</t>
+  </si>
+  <si>
+    <t>The Nug Co.</t>
+  </si>
+  <si>
+    <t>https://peacepipe420.com/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2023/09/30</t>
+  </si>
+  <si>
+    <t>465 BAYLY ST W UNIT 1</t>
+  </si>
+  <si>
+    <t>https://triphouseco.com/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2022/10/14</t>
+  </si>
+  <si>
+    <t>850 WILSON AVE</t>
+  </si>
+  <si>
+    <t>The Trip House</t>
+  </si>
+  <si>
+    <t>https://www.thewoodscannabis.ca/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2023/08/18</t>
+  </si>
+  <si>
+    <t>660 EGLINTON AVE W UNIT 7</t>
+  </si>
+  <si>
+    <t>The Woods Cannabis</t>
+  </si>
+  <si>
+    <t>905-820-5559</t>
+  </si>
+  <si>
+    <t>https://www.thewoodscannabis.ca/dispensary-mississauga</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2023/06/29</t>
+  </si>
+  <si>
+    <t>3145 DUNDAS ST W UNIT 11A</t>
+  </si>
+  <si>
+    <t>https://www.tokecannabis.com/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2021/08/31</t>
+  </si>
+  <si>
+    <t>1133 NOTRE DAME AVE</t>
+  </si>
+  <si>
+    <t>https://ca.tokyosmoke.com/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2023/02/03</t>
+  </si>
+  <si>
+    <t>999 UPPER WENTWORTH ST UNIT 167</t>
+  </si>
+  <si>
+    <t>Tokyo Smoke Lime Ridge Mall</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2023/09/13</t>
+  </si>
+  <si>
+    <t>1355 KINGSTON RD SUITE 71</t>
+  </si>
+  <si>
+    <t>Tokyo Smoke Pickering Town Centre</t>
+  </si>
+  <si>
+    <t>https://ca.tokyosmoke.com/pages/store-locator-1</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2023/10/20</t>
+  </si>
+  <si>
+    <t>925 ONTARIO ST UNIT 5B</t>
+  </si>
+  <si>
+    <t>Tokyo Smoke Stratford Centre</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://www.tweed.com/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">99 MAPLEVIEW DR E UNIT A </t>
+  </si>
+  <si>
+    <t>Tweed</t>
+  </si>
+  <si>
+    <t>https://www.tweed.com/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2021/04/23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">500 GARDINERS ROAD UNIT 2B </t>
+  </si>
+  <si>
+    <t xml:space="preserve">KINGSTON </t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2021/12/22</t>
+  </si>
+  <si>
+    <t>950 LANSDOWNE ST W UNIT A-07</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2022/02/07</t>
+  </si>
+  <si>
+    <t>1970 WALKLEY RD</t>
+  </si>
+  <si>
+    <t>2162 PRINCE OF WALES DR</t>
+  </si>
+  <si>
+    <t>https://locations.timhortons.ca/en/on/burlington/2971-walkers-line/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2022/02/04</t>
+  </si>
+  <si>
+    <t>2971 WALKER'S LINE UNIT A</t>
+  </si>
+  <si>
+    <t>https://twistedterpsdispensary.com/</t>
+  </si>
+  <si>
+    <t>10488 HIGHWAY 7</t>
+  </si>
+  <si>
+    <t>Twisted Terps Cannabis</t>
+  </si>
+  <si>
+    <t>https://uncleherbs.com/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2021/02/19</t>
+  </si>
+  <si>
+    <t>1527 MERIVALE RD</t>
+  </si>
+  <si>
+    <t>UNCLE HERBS CANNABIS</t>
+  </si>
+  <si>
+    <t>https://on.valuebuds.com/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2023/09/06</t>
+  </si>
+  <si>
+    <t>70 FIRST ST</t>
+  </si>
+  <si>
+    <t>https://on.valuebuds.com/pages/search-results-page?collection=value-buds-huron-church-rd</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2023/09/08</t>
+  </si>
+  <si>
+    <t>1726 HURON CHURCH RD SUITE 4</t>
+  </si>
+  <si>
+    <t>['No delivery / Closed']</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2023/07/26</t>
+  </si>
+  <si>
+    <t>2400 DUNDAS ST W UNIT 14</t>
+  </si>
+  <si>
+    <t>WE'D Cannabis</t>
+  </si>
+  <si>
+    <t>1192 THE QUEENSWAY</t>
+  </si>
+  <si>
+    <t>Weed Academy</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2023/10/27</t>
+  </si>
+  <si>
+    <t>234 GRAHAM ROAD</t>
+  </si>
+  <si>
+    <t>West Lorne Leaf</t>
+  </si>
+  <si>
+    <t>WEST LORNE</t>
+  </si>
+  <si>
+    <t>https://yolocan.ca/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2023/11/08</t>
+  </si>
+  <si>
+    <t>168 CURRIE RD</t>
+  </si>
+  <si>
+    <t>Yolo Cannabis</t>
+  </si>
+  <si>
+    <t>DUTTON</t>
+  </si>
+  <si>
+    <t>https://www.zencann.ca/</t>
+  </si>
+  <si>
+    <t>Public Notice Period: Ended 2021/06/17</t>
+  </si>
+  <si>
+    <t>2250 HIGHWAY 7</t>
+  </si>
+  <si>
+    <t>Zen Cannabis</t>
   </si>
 </sst>
 </file>
@@ -11915,10 +12317,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1060"/>
+  <dimension ref="A1:N1099"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1037" workbookViewId="0">
-      <selection activeCell="G1048" sqref="G1048"/>
+    <sheetView tabSelected="1" topLeftCell="A1078" workbookViewId="0">
+      <selection activeCell="F1095" sqref="F1095"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -47090,6 +47492,1176 @@
       </c>
       <c r="J1060" s="33" t="s">
         <v>3650</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1061" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1061" s="1" t="s">
+        <v>3792</v>
+      </c>
+      <c r="C1061" s="1" t="s">
+        <v>3791</v>
+      </c>
+      <c r="D1061" s="11" t="s">
+        <v>3790</v>
+      </c>
+      <c r="E1061" s="32" t="s">
+        <v>3789</v>
+      </c>
+      <c r="F1061" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1061" s="30"/>
+      <c r="H1061" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1061" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1061" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1062" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B1062" s="1" t="s">
+        <v>3796</v>
+      </c>
+      <c r="C1062" s="1" t="s">
+        <v>3795</v>
+      </c>
+      <c r="D1062" s="11" t="s">
+        <v>3794</v>
+      </c>
+      <c r="E1062" s="29" t="s">
+        <v>3793</v>
+      </c>
+      <c r="F1062" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1062" s="30"/>
+      <c r="H1062" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1062" s="31">
+        <v>4162467769</v>
+      </c>
+      <c r="J1062" s="33" t="s">
+        <v>3650</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1063" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B1063" s="1" t="s">
+        <v>3800</v>
+      </c>
+      <c r="C1063" s="1" t="s">
+        <v>3799</v>
+      </c>
+      <c r="D1063" s="11" t="s">
+        <v>3798</v>
+      </c>
+      <c r="E1063" s="29" t="s">
+        <v>3797</v>
+      </c>
+      <c r="F1063" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1063" s="30"/>
+      <c r="H1063" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1063" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1063" s="1" t="s">
+        <v>3534</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1064" s="1" t="s">
+        <v>3286</v>
+      </c>
+      <c r="B1064" s="1" t="s">
+        <v>3804</v>
+      </c>
+      <c r="C1064" s="1" t="s">
+        <v>3803</v>
+      </c>
+      <c r="D1064" s="11" t="s">
+        <v>3802</v>
+      </c>
+      <c r="E1064" s="29" t="s">
+        <v>3801</v>
+      </c>
+      <c r="F1064" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1064" s="30"/>
+      <c r="H1064" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1064" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1064" s="1" t="s">
+        <v>3534</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1065" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1065" s="1" t="s">
+        <v>2785</v>
+      </c>
+      <c r="C1065" s="1" t="s">
+        <v>3807</v>
+      </c>
+      <c r="D1065" s="11" t="s">
+        <v>3806</v>
+      </c>
+      <c r="E1065" s="32" t="s">
+        <v>3805</v>
+      </c>
+      <c r="F1065" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1065" s="30"/>
+      <c r="H1065" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1065" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1065" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1066" s="1" t="s">
+        <v>3812</v>
+      </c>
+      <c r="B1066" s="1" t="s">
+        <v>3811</v>
+      </c>
+      <c r="C1066" s="1" t="s">
+        <v>3810</v>
+      </c>
+      <c r="D1066" s="11" t="s">
+        <v>3809</v>
+      </c>
+      <c r="E1066" s="29" t="s">
+        <v>3808</v>
+      </c>
+      <c r="F1066" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1066" s="30"/>
+      <c r="H1066" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1066" s="31">
+        <v>19016728467</v>
+      </c>
+      <c r="J1066" s="1" t="s">
+        <v>3534</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1067" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1067" s="1" t="s">
+        <v>3815</v>
+      </c>
+      <c r="C1067" s="1" t="s">
+        <v>3814</v>
+      </c>
+      <c r="D1067" s="11" t="s">
+        <v>3813</v>
+      </c>
+      <c r="E1067" s="29" t="s">
+        <v>3540</v>
+      </c>
+      <c r="F1067" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1067" s="30"/>
+      <c r="H1067" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1067" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1067" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1068" s="1" t="s">
+        <v>3142</v>
+      </c>
+      <c r="B1068" s="1" t="s">
+        <v>1324</v>
+      </c>
+      <c r="C1068" s="1" t="s">
+        <v>3818</v>
+      </c>
+      <c r="D1068" s="11" t="s">
+        <v>3817</v>
+      </c>
+      <c r="E1068" s="29" t="s">
+        <v>3816</v>
+      </c>
+      <c r="F1068" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1068" s="30"/>
+      <c r="H1068" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1068" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1068" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1069" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1069" s="1" t="s">
+        <v>3822</v>
+      </c>
+      <c r="C1069" s="1" t="s">
+        <v>3821</v>
+      </c>
+      <c r="D1069" s="11" t="s">
+        <v>3820</v>
+      </c>
+      <c r="E1069" s="32" t="s">
+        <v>3819</v>
+      </c>
+      <c r="F1069" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1069" s="30"/>
+      <c r="H1069" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1069" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1069" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1070" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B1070" s="1" t="s">
+        <v>3824</v>
+      </c>
+      <c r="C1070" s="1" t="s">
+        <v>3823</v>
+      </c>
+      <c r="D1070" s="11" t="s">
+        <v>3480</v>
+      </c>
+      <c r="E1070" s="32" t="s">
+        <v>2923</v>
+      </c>
+      <c r="F1070" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1070" s="30"/>
+      <c r="H1070" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1070" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1070" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1071" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1071" s="1" t="s">
+        <v>3828</v>
+      </c>
+      <c r="C1071" s="1" t="s">
+        <v>3827</v>
+      </c>
+      <c r="D1071" s="11" t="s">
+        <v>3826</v>
+      </c>
+      <c r="E1071" s="32" t="s">
+        <v>3825</v>
+      </c>
+      <c r="F1071" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1071" s="30"/>
+      <c r="H1071" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1071" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1071" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1072" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="B1072" s="1" t="s">
+        <v>3830</v>
+      </c>
+      <c r="C1072" s="1" t="s">
+        <v>3829</v>
+      </c>
+      <c r="D1072" s="11" t="s">
+        <v>3652</v>
+      </c>
+      <c r="E1072" s="32" t="s">
+        <v>981</v>
+      </c>
+      <c r="F1072" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1072" s="30"/>
+      <c r="H1072" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1072" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1072" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1073" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1073" s="1" t="s">
+        <v>3834</v>
+      </c>
+      <c r="C1073" s="1" t="s">
+        <v>3833</v>
+      </c>
+      <c r="D1073" s="11" t="s">
+        <v>3832</v>
+      </c>
+      <c r="E1073" s="29" t="s">
+        <v>3831</v>
+      </c>
+      <c r="F1073" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1073" s="30"/>
+      <c r="H1073" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1073" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1073" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1074" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1074" s="1" t="s">
+        <v>3838</v>
+      </c>
+      <c r="C1074" s="1" t="s">
+        <v>3837</v>
+      </c>
+      <c r="D1074" s="11" t="s">
+        <v>3836</v>
+      </c>
+      <c r="E1074" s="32" t="s">
+        <v>3835</v>
+      </c>
+      <c r="F1074" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1074" s="30"/>
+      <c r="H1074" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1074" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1074" s="33" t="s">
+        <v>3478</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1075" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1075" s="1" t="s">
+        <v>2799</v>
+      </c>
+      <c r="C1075" s="1" t="s">
+        <v>3841</v>
+      </c>
+      <c r="D1075" s="11" t="s">
+        <v>3840</v>
+      </c>
+      <c r="E1075" s="32" t="s">
+        <v>3839</v>
+      </c>
+      <c r="F1075" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1075" s="30"/>
+      <c r="H1075" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1075" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1075" s="33" t="s">
+        <v>3478</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1076" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B1076" s="1" t="s">
+        <v>3846</v>
+      </c>
+      <c r="C1076" s="1" t="s">
+        <v>3845</v>
+      </c>
+      <c r="D1076" s="11" t="s">
+        <v>3844</v>
+      </c>
+      <c r="E1076" s="29" t="s">
+        <v>3843</v>
+      </c>
+      <c r="F1076" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1076" s="30"/>
+      <c r="H1076" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1076" s="31">
+        <v>19052420647</v>
+      </c>
+      <c r="J1076" s="33" t="s">
+        <v>3842</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1077" s="1" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B1077" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1077" s="1" t="s">
+        <v>3849</v>
+      </c>
+      <c r="D1077" s="11" t="s">
+        <v>3848</v>
+      </c>
+      <c r="E1077" s="29" t="s">
+        <v>3847</v>
+      </c>
+      <c r="F1077" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1077" s="30"/>
+      <c r="H1077" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1077" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1077" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1078" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1078" s="1" t="s">
+        <v>3853</v>
+      </c>
+      <c r="C1078" s="1" t="s">
+        <v>3852</v>
+      </c>
+      <c r="D1078" s="11" t="s">
+        <v>3851</v>
+      </c>
+      <c r="E1078" s="32" t="s">
+        <v>3850</v>
+      </c>
+      <c r="F1078" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1078" s="30"/>
+      <c r="H1078" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1078" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1078" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1079" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B1079" s="1" t="s">
+        <v>3857</v>
+      </c>
+      <c r="C1079" s="1" t="s">
+        <v>3856</v>
+      </c>
+      <c r="D1079" s="11" t="s">
+        <v>3855</v>
+      </c>
+      <c r="E1079" s="32" t="s">
+        <v>3854</v>
+      </c>
+      <c r="F1079" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1079" s="30"/>
+      <c r="H1079" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1079" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1079" s="33" t="s">
+        <v>3579</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1080" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B1080" s="1" t="s">
+        <v>3857</v>
+      </c>
+      <c r="C1080" s="1" t="s">
+        <v>3861</v>
+      </c>
+      <c r="D1080" s="11" t="s">
+        <v>3860</v>
+      </c>
+      <c r="E1080" s="29" t="s">
+        <v>3859</v>
+      </c>
+      <c r="F1080" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1080" s="30"/>
+      <c r="H1080" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1080" s="31" t="s">
+        <v>3858</v>
+      </c>
+      <c r="J1080" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1081" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="B1081" s="1" t="s">
+        <v>3328</v>
+      </c>
+      <c r="C1081" s="1" t="s">
+        <v>3864</v>
+      </c>
+      <c r="D1081" s="11" t="s">
+        <v>3863</v>
+      </c>
+      <c r="E1081" s="32" t="s">
+        <v>3862</v>
+      </c>
+      <c r="F1081" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1081" s="30"/>
+      <c r="H1081" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1081" s="31">
+        <v>17052073887</v>
+      </c>
+      <c r="J1081" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1082" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1082" s="1" t="s">
+        <v>3868</v>
+      </c>
+      <c r="C1082" s="1" t="s">
+        <v>3867</v>
+      </c>
+      <c r="D1082" s="11" t="s">
+        <v>3866</v>
+      </c>
+      <c r="E1082" s="29" t="s">
+        <v>3865</v>
+      </c>
+      <c r="F1082" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1082" s="30"/>
+      <c r="H1082" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1082" s="31">
+        <v>19053874455</v>
+      </c>
+      <c r="J1082" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1083" s="1" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B1083" s="1" t="s">
+        <v>3871</v>
+      </c>
+      <c r="C1083" s="1" t="s">
+        <v>3870</v>
+      </c>
+      <c r="D1083" s="11" t="s">
+        <v>3869</v>
+      </c>
+      <c r="E1083" s="29" t="s">
+        <v>3865</v>
+      </c>
+      <c r="F1083" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1083" s="30"/>
+      <c r="H1083" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1083" s="31">
+        <v>19056837171</v>
+      </c>
+      <c r="J1083" s="1" t="s">
+        <v>3534</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1084" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B1084" s="1" t="s">
+        <v>3875</v>
+      </c>
+      <c r="C1084" s="1" t="s">
+        <v>3874</v>
+      </c>
+      <c r="D1084" s="11" t="s">
+        <v>3873</v>
+      </c>
+      <c r="E1084" s="29" t="s">
+        <v>3872</v>
+      </c>
+      <c r="F1084" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1084" s="30"/>
+      <c r="H1084" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1084" s="10">
+        <v>15195081925</v>
+      </c>
+      <c r="J1084" s="1" t="s">
+        <v>3534</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1085" s="1" t="s">
+        <v>676</v>
+      </c>
+      <c r="B1085" s="1" t="s">
+        <v>3878</v>
+      </c>
+      <c r="C1085" s="1" t="s">
+        <v>3877</v>
+      </c>
+      <c r="D1085" s="11" t="s">
+        <v>3678</v>
+      </c>
+      <c r="E1085" s="29" t="s">
+        <v>3876</v>
+      </c>
+      <c r="F1085" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1085" s="30"/>
+      <c r="H1085" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1085" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1085" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1086" s="1" t="s">
+        <v>3882</v>
+      </c>
+      <c r="B1086" s="1" t="s">
+        <v>3878</v>
+      </c>
+      <c r="C1086" s="1" t="s">
+        <v>3881</v>
+      </c>
+      <c r="D1086" s="11" t="s">
+        <v>3880</v>
+      </c>
+      <c r="E1086" s="29" t="s">
+        <v>3879</v>
+      </c>
+      <c r="F1086" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1086" s="30"/>
+      <c r="H1086" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1086" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1086" s="33" t="s">
+        <v>3478</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1087" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1087" s="1" t="s">
+        <v>3878</v>
+      </c>
+      <c r="C1087" s="1" t="s">
+        <v>3884</v>
+      </c>
+      <c r="D1087" s="11" t="s">
+        <v>3883</v>
+      </c>
+      <c r="E1087" s="32" t="s">
+        <v>3879</v>
+      </c>
+      <c r="F1087" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1087" s="30"/>
+      <c r="H1087" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1087" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1087" s="33" t="s">
+        <v>3579</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1088" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1088" s="1" t="s">
+        <v>3878</v>
+      </c>
+      <c r="C1088" s="1" t="s">
+        <v>3886</v>
+      </c>
+      <c r="D1088" s="11" t="s">
+        <v>3885</v>
+      </c>
+      <c r="E1088" s="29" t="s">
+        <v>3879</v>
+      </c>
+      <c r="F1088" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1088" s="30"/>
+      <c r="H1088" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1088" s="31">
+        <v>16135219090</v>
+      </c>
+      <c r="J1088" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1089" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B1089" s="1" t="s">
+        <v>3878</v>
+      </c>
+      <c r="C1089" s="1" t="s">
+        <v>3887</v>
+      </c>
+      <c r="D1089" s="11" t="s">
+        <v>3885</v>
+      </c>
+      <c r="E1089" s="29" t="s">
+        <v>3879</v>
+      </c>
+      <c r="F1089" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1089" s="30"/>
+      <c r="H1089" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1089" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1089" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1090" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1090" s="1" t="s">
+        <v>3878</v>
+      </c>
+      <c r="C1090" s="1" t="s">
+        <v>3890</v>
+      </c>
+      <c r="D1090" s="11" t="s">
+        <v>3889</v>
+      </c>
+      <c r="E1090" s="29" t="s">
+        <v>3888</v>
+      </c>
+      <c r="F1090" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1090" s="30"/>
+      <c r="H1090" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1090" s="31">
+        <v>19053325355</v>
+      </c>
+      <c r="J1090" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1091" s="1" t="s">
+        <v>2423</v>
+      </c>
+      <c r="B1091" s="1" t="s">
+        <v>3893</v>
+      </c>
+      <c r="C1091" s="1" t="s">
+        <v>3892</v>
+      </c>
+      <c r="D1091" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="E1091" s="29" t="s">
+        <v>3891</v>
+      </c>
+      <c r="F1091" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1091" s="30"/>
+      <c r="H1091" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1091" s="31">
+        <v>19363559752</v>
+      </c>
+      <c r="J1091" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1092" s="1" t="s">
+        <v>538</v>
+      </c>
+      <c r="B1092" s="1" t="s">
+        <v>3897</v>
+      </c>
+      <c r="C1092" s="1" t="s">
+        <v>3896</v>
+      </c>
+      <c r="D1092" s="11" t="s">
+        <v>3895</v>
+      </c>
+      <c r="E1092" s="32" t="s">
+        <v>3894</v>
+      </c>
+      <c r="F1092" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1092" s="30"/>
+      <c r="H1092" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1092" s="31">
+        <v>6137274567</v>
+      </c>
+      <c r="J1092" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1093" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="B1093" s="1" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C1093" s="1" t="s">
+        <v>3900</v>
+      </c>
+      <c r="D1093" s="11" t="s">
+        <v>3899</v>
+      </c>
+      <c r="E1093" s="29" t="s">
+        <v>3898</v>
+      </c>
+      <c r="F1093" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1093" s="30"/>
+      <c r="H1093" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1093" s="31">
+        <v>14163642321</v>
+      </c>
+      <c r="J1093" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1094" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1094" s="1" t="s">
+        <v>1429</v>
+      </c>
+      <c r="C1094" s="1" t="s">
+        <v>3903</v>
+      </c>
+      <c r="D1094" s="11" t="s">
+        <v>3902</v>
+      </c>
+      <c r="E1094" s="32" t="s">
+        <v>3901</v>
+      </c>
+      <c r="F1094" s="6" t="s">
+        <v>1355</v>
+      </c>
+      <c r="G1094" s="30"/>
+      <c r="H1094" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1094" s="31">
+        <v>15192549933</v>
+      </c>
+      <c r="J1094" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1095" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="B1095" s="1" t="s">
+        <v>3907</v>
+      </c>
+      <c r="C1095" s="1" t="s">
+        <v>3906</v>
+      </c>
+      <c r="D1095" s="11" t="s">
+        <v>3905</v>
+      </c>
+      <c r="E1095" s="29" t="s">
+        <v>2345</v>
+      </c>
+      <c r="F1095" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1095" s="30"/>
+      <c r="H1095" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1095" s="31">
+        <v>12896749333</v>
+      </c>
+      <c r="J1095" s="33" t="s">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1096" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1096" s="1" t="s">
+        <v>3909</v>
+      </c>
+      <c r="C1096" s="1" t="s">
+        <v>3908</v>
+      </c>
+      <c r="D1096" s="11" t="s">
+        <v>3776</v>
+      </c>
+      <c r="E1096" s="29" t="s">
+        <v>3540</v>
+      </c>
+      <c r="F1096" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1096" s="30"/>
+      <c r="H1096" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1096" s="31" t="s">
+        <v>3539</v>
+      </c>
+      <c r="J1096" s="33" t="s">
+        <v>3478</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1097" s="1" t="s">
+        <v>3913</v>
+      </c>
+      <c r="B1097" s="1" t="s">
+        <v>3912</v>
+      </c>
+      <c r="C1097" s="1" t="s">
+        <v>3911</v>
+      </c>
+      <c r="D1097" s="11" t="s">
+        <v>3910</v>
+      </c>
+      <c r="E1097" s="29" t="s">
+        <v>3540</v>
+      </c>
+      <c r="F1097" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1097" s="30"/>
+      <c r="H1097" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1097" s="31">
+        <v>5197682620</v>
+      </c>
+      <c r="J1097" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1098" s="1" t="s">
+        <v>3918</v>
+      </c>
+      <c r="B1098" s="1" t="s">
+        <v>3917</v>
+      </c>
+      <c r="C1098" s="1" t="s">
+        <v>3916</v>
+      </c>
+      <c r="D1098" s="11" t="s">
+        <v>3915</v>
+      </c>
+      <c r="E1098" s="29" t="s">
+        <v>3914</v>
+      </c>
+      <c r="F1098" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1098" s="30"/>
+      <c r="H1098" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1098" s="31">
+        <v>15197626262</v>
+      </c>
+      <c r="J1098" s="1" t="s">
+        <v>3461</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1099" s="1" t="s">
+        <v>1741</v>
+      </c>
+      <c r="B1099" s="1" t="s">
+        <v>3922</v>
+      </c>
+      <c r="C1099" s="1" t="s">
+        <v>3921</v>
+      </c>
+      <c r="D1099" s="11" t="s">
+        <v>3920</v>
+      </c>
+      <c r="E1099" s="29" t="s">
+        <v>3919</v>
+      </c>
+      <c r="F1099" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1099" s="30"/>
+      <c r="H1099" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1099" s="31">
+        <v>15197429366</v>
+      </c>
+      <c r="J1099" s="1" t="s">
+        <v>3461</v>
       </c>
     </row>
   </sheetData>
@@ -47129,9 +48701,22 @@
     <hyperlink ref="E1053" r:id="rId33"/>
     <hyperlink ref="E1059" r:id="rId34"/>
     <hyperlink ref="I1060" r:id="rId35" display="tel: 905-896-7756"/>
+    <hyperlink ref="E1061" r:id="rId36"/>
+    <hyperlink ref="E1065" r:id="rId37"/>
+    <hyperlink ref="E1069" r:id="rId38"/>
+    <hyperlink ref="E1070" r:id="rId39"/>
+    <hyperlink ref="E1071" r:id="rId40"/>
+    <hyperlink ref="E1072" r:id="rId41"/>
+    <hyperlink ref="E1075" r:id="rId42"/>
+    <hyperlink ref="E1078" r:id="rId43"/>
+    <hyperlink ref="E1079" r:id="rId44"/>
+    <hyperlink ref="E1081" r:id="rId45"/>
+    <hyperlink ref="I1084" r:id="rId46" display="tel:+15195081925"/>
+    <hyperlink ref="E1087" r:id="rId47"/>
+    <hyperlink ref="E1092" r:id="rId48"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId36"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId49"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
save new data - 1322
</commit_message>
<xml_diff>
--- a/platform_scrapper/CANNABIS_RESULTS/found_IDs.xlsx
+++ b/platform_scrapper/CANNABIS_RESULTS/found_IDs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11343" uniqueCount="4481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11589" uniqueCount="4569">
   <si>
     <t>BURLINGTON</t>
   </si>
@@ -13459,13 +13459,277 @@
   </si>
   <si>
     <t>RIDGEBURN</t>
+  </si>
+  <si>
+    <t>606df11e89f0224278fb8e7a</t>
+  </si>
+  <si>
+    <t>http://www.purplemeadow.ca/</t>
+  </si>
+  <si>
+    <t>2059 MEADOWBROOK RD</t>
+  </si>
+  <si>
+    <t>Purple Meadow Cannabis</t>
+  </si>
+  <si>
+    <t>http://www.tribalnationflowerco.com/</t>
+  </si>
+  <si>
+    <t>10166 GLENDON DR UNIT 204</t>
+  </si>
+  <si>
+    <t>Inspired Cannabis Co</t>
+  </si>
+  <si>
+    <t>KOMOKA</t>
+  </si>
+  <si>
+    <t>['No delivery / closed']</t>
+  </si>
+  <si>
+    <t>http://www.purplecircle.ca/</t>
+  </si>
+  <si>
+    <t>21A CARLTON ST</t>
+  </si>
+  <si>
+    <t>Purple Circle Cannabis</t>
+  </si>
+  <si>
+    <t>http://www.southriverbuds.ca/</t>
+  </si>
+  <si>
+    <t>19 ISABELLA STREET</t>
+  </si>
+  <si>
+    <t>South River Buds</t>
+  </si>
+  <si>
+    <t>SOUTH RIVER</t>
+  </si>
+  <si>
+    <t>61294e2fb96abc00aa15da74</t>
+  </si>
+  <si>
+    <t>http://www.spiritleaf.ca/</t>
+  </si>
+  <si>
+    <t>1750 THE QUEENSWAY UNIT 5</t>
+  </si>
+  <si>
+    <t>5e8c9c757b2d2700bdc6939e</t>
+  </si>
+  <si>
+    <t>2389 BLOOR ST W</t>
+  </si>
+  <si>
+    <t>354 ROYAL YORK RD</t>
+  </si>
+  <si>
+    <t>http://www.springscannabis.ca/</t>
+  </si>
+  <si>
+    <t>692 UPPER JAMES ST UNIT B</t>
+  </si>
+  <si>
+    <t>Spring cannabis express</t>
+  </si>
+  <si>
+    <t>5f9983b35d129e00b8daaa7c</t>
+  </si>
+  <si>
+    <t>171 FORT YORK BLVD</t>
+  </si>
+  <si>
+    <t>STICKY NUGGZ FORT YORK</t>
+  </si>
+  <si>
+    <t>http://www.stirlingcannabis.ca/</t>
+  </si>
+  <si>
+    <t>28 MILL STREET</t>
+  </si>
+  <si>
+    <t>STIRLING CANNABIS</t>
+  </si>
+  <si>
+    <t>http://www.shopstrictly.ca/</t>
+  </si>
+  <si>
+    <t>3351 MARKHAM RD SUITE 136</t>
+  </si>
+  <si>
+    <t>Strictly Cannabis</t>
+  </si>
+  <si>
+    <t>http://www.sunfishcannabis.com/</t>
+  </si>
+  <si>
+    <t>112 QUEEN ST, UNIT #2</t>
+  </si>
+  <si>
+    <t>SunFish Cannabis</t>
+  </si>
+  <si>
+    <t>LAKEFIELD</t>
+  </si>
+  <si>
+    <t>30 OTTAWA STREET, EAST UNIT</t>
+  </si>
+  <si>
+    <t>Sunfish Cannabis Trainstation</t>
+  </si>
+  <si>
+    <t>HAVELOCK</t>
+  </si>
+  <si>
+    <t>638f938672811000d58b0b83</t>
+  </si>
+  <si>
+    <t>http://www.tosmoke.ca/</t>
+  </si>
+  <si>
+    <t>2432 EGLINTON AVE E</t>
+  </si>
+  <si>
+    <t>T.O. Smokes</t>
+  </si>
+  <si>
+    <t>5fb58bff804afc00d8cc12c0</t>
+  </si>
+  <si>
+    <t>http://www.thecannabisconnoisseur.ca/</t>
+  </si>
+  <si>
+    <t>1874 SCUGOG ST UNIT 2</t>
+  </si>
+  <si>
+    <t>The Cannabis Connoisseur</t>
+  </si>
+  <si>
+    <t>60ef45404665d400b093949e</t>
+  </si>
+  <si>
+    <t>http://www.theherbary.com/</t>
+  </si>
+  <si>
+    <t>1650 BATH RD</t>
+  </si>
+  <si>
+    <t>61eafd3db150740085dd5336</t>
+  </si>
+  <si>
+    <t>233 VICTORIA ST N UNIT 1</t>
+  </si>
+  <si>
+    <t>OLYMPIA CANNABIS TWEED (O/C TWEED)</t>
+  </si>
+  <si>
+    <t>http://www.unplugcannabis.com/</t>
+  </si>
+  <si>
+    <t>4055 CARLING AVE UNIT 4</t>
+  </si>
+  <si>
+    <t>Unplug Cannabis Co.</t>
+  </si>
+  <si>
+    <t>1375 TRIM RD UNIT 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">261 RICHMOND ROAD  </t>
+  </si>
+  <si>
+    <t>5fd91fe986dbe500b1c3b576</t>
+  </si>
+  <si>
+    <t>http://www.tonikcannabis.com/</t>
+  </si>
+  <si>
+    <t>560 WEST ST SUITE B</t>
+  </si>
+  <si>
+    <t>TONIK CANNABIS</t>
+  </si>
+  <si>
+    <t>6112948df8b18200c5194f6f</t>
+  </si>
+  <si>
+    <t>http://www.tokehouse.ca/dryden</t>
+  </si>
+  <si>
+    <t>539 GOVERNMENT ST UNIT 16</t>
+  </si>
+  <si>
+    <t>['No delivery / CLosed']</t>
+  </si>
+  <si>
+    <t>http://www.tokeandtell.ca/</t>
+  </si>
+  <si>
+    <t>184 WILSON AVE</t>
+  </si>
+  <si>
+    <t>TOKE AND TELL CANNABIS</t>
+  </si>
+  <si>
+    <t>618a8a4374a28f007712ff0a</t>
+  </si>
+  <si>
+    <t>http://www.tokacannabis.com/</t>
+  </si>
+  <si>
+    <t>490 CHRYSLER DR SUITE 49</t>
+  </si>
+  <si>
+    <t>TOKA+</t>
+  </si>
+  <si>
+    <t>60257bc9b754e700e41f5acc</t>
+  </si>
+  <si>
+    <t>http://www.thisel.ca/</t>
+  </si>
+  <si>
+    <t>192 QUEEN'S QUAY EAST UNIT A5</t>
+  </si>
+  <si>
+    <t>THISEL</t>
+  </si>
+  <si>
+    <t>60f6fa3f34269200b8673d58</t>
+  </si>
+  <si>
+    <t>1301 RICHMOND RD</t>
+  </si>
+  <si>
+    <t>http://www.thehappycannasseur.com/</t>
+  </si>
+  <si>
+    <t>1413 KING ST E UNIT 5</t>
+  </si>
+  <si>
+    <t>The Happy Cannasseur</t>
+  </si>
+  <si>
+    <t>http://www.thegreenbouquet.ca/</t>
+  </si>
+  <si>
+    <t>15 SOUTH MARY LAKE RD UNIT 2</t>
+  </si>
+  <si>
+    <t>The Green Bouquet Cannabis</t>
+  </si>
+  <si>
+    <t>PORT SYDNEY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -13579,8 +13843,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -13607,12 +13878,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -13646,7 +13911,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
@@ -13700,18 +13965,15 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="11" fontId="10" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
@@ -14015,10 +14277,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1294"/>
+  <dimension ref="A1:N1323"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1272" workbookViewId="0">
-      <selection activeCell="C1294" sqref="C1294"/>
+    <sheetView tabSelected="1" topLeftCell="A1297" workbookViewId="0">
+      <selection activeCell="C1304" sqref="C1304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -55463,7 +55725,7 @@
       <c r="F1258" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1258" s="41" t="s">
+      <c r="G1258" s="37" t="s">
         <v>4369</v>
       </c>
       <c r="H1258" s="1" t="s">
@@ -55490,7 +55752,7 @@
       <c r="D1259" s="11" t="s">
         <v>4371</v>
       </c>
-      <c r="E1259" s="36" t="s">
+      <c r="E1259" s="33" t="s">
         <v>1904</v>
       </c>
       <c r="F1259" s="6" t="s">
@@ -55526,10 +55788,10 @@
       <c r="E1260" s="29" t="s">
         <v>4245</v>
       </c>
-      <c r="F1260" s="38" t="s">
+      <c r="F1260" s="6" t="s">
         <v>4375</v>
       </c>
-      <c r="G1260" s="37" t="s">
+      <c r="G1260" s="34" t="s">
         <v>4373</v>
       </c>
       <c r="H1260" s="1" t="s">
@@ -55541,101 +55803,101 @@
       <c r="J1260" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N1260" s="12"/>
-    </row>
-    <row r="1261" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1261" t="s">
+      <c r="N1260" s="38"/>
+    </row>
+    <row r="1261" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1261" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1261" t="s">
+      <c r="B1261" s="1" t="s">
         <v>4379</v>
       </c>
-      <c r="C1261" t="s">
+      <c r="C1261" s="1" t="s">
         <v>4378</v>
       </c>
-      <c r="D1261" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1261" s="34" t="s">
+      <c r="D1261" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1261" s="29" t="s">
         <v>4377</v>
       </c>
-      <c r="F1261" s="38" t="s">
+      <c r="F1261" s="6" t="s">
         <v>4375</v>
       </c>
-      <c r="G1261" s="42" t="s">
+      <c r="G1261" s="37" t="s">
         <v>4376</v>
       </c>
-      <c r="H1261" t="s">
+      <c r="H1261" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I1261">
+      <c r="I1261" s="1">
         <v>14165193487</v>
       </c>
-      <c r="J1261" s="4" t="s">
+      <c r="J1261" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="1262" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1262" t="s">
+    <row r="1262" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1262" s="1" t="s">
         <v>2336</v>
       </c>
-      <c r="B1262" t="s">
+      <c r="B1262" s="1" t="s">
         <v>1953</v>
       </c>
-      <c r="C1262" t="s">
+      <c r="C1262" s="1" t="s">
         <v>4381</v>
       </c>
-      <c r="D1262" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1262" s="34" t="s">
+      <c r="D1262" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1262" s="29" t="s">
         <v>2320</v>
       </c>
-      <c r="F1262" s="38" t="s">
+      <c r="F1262" s="6" t="s">
         <v>4375</v>
       </c>
-      <c r="G1262" s="35" t="s">
+      <c r="G1262" s="31" t="s">
         <v>4380</v>
       </c>
-      <c r="H1262" t="s">
+      <c r="H1262" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="I1262">
+      <c r="I1262" s="1">
         <v>19055635255</v>
       </c>
-      <c r="J1262" t="s">
+      <c r="J1262" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="1263" spans="1:14" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1263" t="s">
+    <row r="1263" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1263" s="1" t="s">
         <v>998</v>
       </c>
-      <c r="B1263" t="s">
+      <c r="B1263" s="1" t="s">
         <v>1953</v>
       </c>
-      <c r="C1263" t="s">
+      <c r="C1263" s="1" t="s">
         <v>4383</v>
       </c>
-      <c r="D1263" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1263" s="34" t="s">
+      <c r="D1263" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1263" s="29" t="s">
         <v>2320</v>
       </c>
-      <c r="F1263" s="33" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1263" s="42" t="s">
+      <c r="F1263" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1263" s="37" t="s">
         <v>4382</v>
       </c>
-      <c r="H1263" t="s">
+      <c r="H1263" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I1263">
+      <c r="I1263" s="1">
         <v>17056288828</v>
       </c>
-      <c r="J1263" t="s">
+      <c r="J1263" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -55658,7 +55920,7 @@
       <c r="F1264" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1264" s="41" t="s">
+      <c r="G1264" s="37" t="s">
         <v>4376</v>
       </c>
       <c r="H1264" s="1" t="s">
@@ -55722,7 +55984,7 @@
       <c r="F1266" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1266" s="41" t="s">
+      <c r="G1266" s="37" t="s">
         <v>4387</v>
       </c>
       <c r="H1266" s="1" t="s">
@@ -55755,7 +56017,7 @@
       <c r="F1267" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1267" s="41" t="s">
+      <c r="G1267" s="37" t="s">
         <v>4391</v>
       </c>
       <c r="H1267" s="1" t="s">
@@ -55788,7 +56050,7 @@
       <c r="F1268" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1268" s="41" t="s">
+      <c r="G1268" s="37" t="s">
         <v>4395</v>
       </c>
       <c r="H1268" s="1" t="s">
@@ -55914,7 +56176,7 @@
       <c r="F1272" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1272" s="39" t="s">
+      <c r="G1272" s="35" t="s">
         <v>4408</v>
       </c>
       <c r="H1272" s="1" t="s">
@@ -56009,7 +56271,7 @@
       <c r="F1275" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1275" s="40" t="s">
+      <c r="G1275" s="36" t="s">
         <v>4418</v>
       </c>
       <c r="H1275" s="1" t="s">
@@ -56075,7 +56337,7 @@
       <c r="F1277" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1277" s="37" t="s">
+      <c r="G1277" s="34" t="s">
         <v>4426</v>
       </c>
       <c r="H1277" s="1" t="s">
@@ -56265,7 +56527,7 @@
       <c r="F1283" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1283" s="40" t="s">
+      <c r="G1283" s="36" t="s">
         <v>4440</v>
       </c>
       <c r="H1283" s="1" t="s">
@@ -56593,6 +56855,7 @@
       <c r="J1293" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="N1293" s="12"/>
     </row>
     <row r="1294" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1294" s="1" t="s">
@@ -56613,7 +56876,7 @@
       <c r="F1294" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G1294" s="41" t="s">
+      <c r="G1294" s="37" t="s">
         <v>4477</v>
       </c>
       <c r="H1294" s="1" t="s">
@@ -56624,6 +56887,921 @@
       </c>
       <c r="J1294" s="1" t="s">
         <v>8</v>
+      </c>
+      <c r="N1294" s="12"/>
+    </row>
+    <row r="1295" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1295" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="B1295" s="1" t="s">
+        <v>4484</v>
+      </c>
+      <c r="C1295" s="1" t="s">
+        <v>4483</v>
+      </c>
+      <c r="D1295" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1295" s="29" t="s">
+        <v>4482</v>
+      </c>
+      <c r="F1295" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1295" s="37" t="s">
+        <v>4481</v>
+      </c>
+      <c r="H1295" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="I1295" s="1">
+        <v>16138429333</v>
+      </c>
+      <c r="J1295" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1295" s="12"/>
+    </row>
+    <row r="1296" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1296" s="1" t="s">
+        <v>4488</v>
+      </c>
+      <c r="B1296" s="1" t="s">
+        <v>4487</v>
+      </c>
+      <c r="C1296" s="1" t="s">
+        <v>4486</v>
+      </c>
+      <c r="D1296" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1296" s="29" t="s">
+        <v>4485</v>
+      </c>
+      <c r="F1296" s="6" t="s">
+        <v>1448</v>
+      </c>
+      <c r="G1296" s="31"/>
+      <c r="H1296" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1296" s="1">
+        <v>15597156979</v>
+      </c>
+      <c r="J1296" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1296" s="12"/>
+    </row>
+    <row r="1297" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1297" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1297" s="1" t="s">
+        <v>4492</v>
+      </c>
+      <c r="C1297" s="1" t="s">
+        <v>4491</v>
+      </c>
+      <c r="D1297" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1297" s="29" t="s">
+        <v>4490</v>
+      </c>
+      <c r="F1297" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1297" s="31"/>
+      <c r="H1297" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1297" s="1">
+        <v>14163990995</v>
+      </c>
+      <c r="J1297" s="1" t="s">
+        <v>4489</v>
+      </c>
+      <c r="N1297" s="12"/>
+    </row>
+    <row r="1298" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1298" s="1" t="s">
+        <v>4496</v>
+      </c>
+      <c r="B1298" s="1" t="s">
+        <v>4495</v>
+      </c>
+      <c r="C1298" s="1" t="s">
+        <v>4494</v>
+      </c>
+      <c r="D1298" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1298" s="29" t="s">
+        <v>4493</v>
+      </c>
+      <c r="F1298" s="6" t="s">
+        <v>4108</v>
+      </c>
+      <c r="G1298" s="31"/>
+      <c r="H1298" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1298" s="1">
+        <v>17053861264</v>
+      </c>
+      <c r="J1298" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1298" s="12"/>
+    </row>
+    <row r="1299" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1299" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1299" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1299" s="1" t="s">
+        <v>4499</v>
+      </c>
+      <c r="D1299" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1299" s="29" t="s">
+        <v>4498</v>
+      </c>
+      <c r="F1299" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1299" s="39" t="s">
+        <v>4497</v>
+      </c>
+      <c r="H1299" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1299" s="1">
+        <v>14165193555</v>
+      </c>
+      <c r="J1299" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1299" s="12"/>
+    </row>
+    <row r="1300" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1300" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1300" s="1" t="s">
+        <v>534</v>
+      </c>
+      <c r="C1300" s="1" t="s">
+        <v>4501</v>
+      </c>
+      <c r="D1300" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1300" s="29" t="s">
+        <v>4498</v>
+      </c>
+      <c r="F1300" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1300" s="39" t="s">
+        <v>4500</v>
+      </c>
+      <c r="H1300" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1300" s="1">
+        <v>14167672225</v>
+      </c>
+      <c r="J1300" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1300" s="12"/>
+    </row>
+    <row r="1301" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1301" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1301" s="1" t="s">
+        <v>3796</v>
+      </c>
+      <c r="C1301" s="1" t="s">
+        <v>4502</v>
+      </c>
+      <c r="D1301" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="E1301" s="29" t="s">
+        <v>3793</v>
+      </c>
+      <c r="F1301" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1301" s="31"/>
+      <c r="H1301" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1301" s="1">
+        <v>14162557768</v>
+      </c>
+      <c r="J1301" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1301" s="12"/>
+    </row>
+    <row r="1302" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1302" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1302" s="1" t="s">
+        <v>4505</v>
+      </c>
+      <c r="C1302" s="1" t="s">
+        <v>4504</v>
+      </c>
+      <c r="D1302" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1302" s="29" t="s">
+        <v>4503</v>
+      </c>
+      <c r="F1302" s="6" t="s">
+        <v>560</v>
+      </c>
+      <c r="G1302" s="31"/>
+      <c r="H1302" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1302" s="1">
+        <v>19055193589</v>
+      </c>
+      <c r="J1302" s="1" t="s">
+        <v>3478</v>
+      </c>
+      <c r="N1302" s="12"/>
+    </row>
+    <row r="1303" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1303" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1303" s="1" t="s">
+        <v>4508</v>
+      </c>
+      <c r="C1303" s="1" t="s">
+        <v>4507</v>
+      </c>
+      <c r="D1303" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1303" s="29" t="s">
+        <v>3797</v>
+      </c>
+      <c r="F1303" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1303" s="39" t="s">
+        <v>4506</v>
+      </c>
+      <c r="H1303" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1303" s="1">
+        <v>14168678888</v>
+      </c>
+      <c r="J1303" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1303" s="12"/>
+    </row>
+    <row r="1304" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1304" s="1" t="s">
+        <v>1941</v>
+      </c>
+      <c r="B1304" s="1" t="s">
+        <v>4511</v>
+      </c>
+      <c r="C1304" s="1" t="s">
+        <v>4510</v>
+      </c>
+      <c r="D1304" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1304" s="29" t="s">
+        <v>4509</v>
+      </c>
+      <c r="F1304" s="6" t="s">
+        <v>1650</v>
+      </c>
+      <c r="G1304" s="31"/>
+      <c r="H1304" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1304" s="1">
+        <v>16133952223</v>
+      </c>
+      <c r="J1304" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1304" s="12"/>
+    </row>
+    <row r="1305" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1305" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1305" s="1" t="s">
+        <v>4514</v>
+      </c>
+      <c r="C1305" s="1" t="s">
+        <v>4513</v>
+      </c>
+      <c r="D1305" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1305" s="29" t="s">
+        <v>4512</v>
+      </c>
+      <c r="F1305" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1305" s="31"/>
+      <c r="H1305" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1305" s="1">
+        <v>14162664420</v>
+      </c>
+      <c r="J1305" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1305" s="12"/>
+    </row>
+    <row r="1306" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1306" s="1" t="s">
+        <v>4518</v>
+      </c>
+      <c r="B1306" s="1" t="s">
+        <v>4517</v>
+      </c>
+      <c r="C1306" s="1" t="s">
+        <v>4516</v>
+      </c>
+      <c r="D1306" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1306" s="29" t="s">
+        <v>4515</v>
+      </c>
+      <c r="F1306" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1306" s="31"/>
+      <c r="H1306" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1306" s="1">
+        <v>17056513474</v>
+      </c>
+      <c r="J1306" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1306" s="12"/>
+    </row>
+    <row r="1307" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1307" s="1" t="s">
+        <v>4521</v>
+      </c>
+      <c r="B1307" s="1" t="s">
+        <v>4520</v>
+      </c>
+      <c r="C1307" s="1" t="s">
+        <v>4519</v>
+      </c>
+      <c r="D1307" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1307" s="30" t="s">
+        <v>4515</v>
+      </c>
+      <c r="F1307" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1307" s="31"/>
+      <c r="H1307" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1307" s="1">
+        <v>17056513474</v>
+      </c>
+      <c r="J1307" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1307" s="12"/>
+    </row>
+    <row r="1308" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1308" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="B1308" s="1" t="s">
+        <v>4525</v>
+      </c>
+      <c r="C1308" s="1" t="s">
+        <v>4524</v>
+      </c>
+      <c r="D1308" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1308" s="29" t="s">
+        <v>4523</v>
+      </c>
+      <c r="F1308" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1308" s="39" t="s">
+        <v>4522</v>
+      </c>
+      <c r="H1308" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1308" s="1">
+        <v>14167524242</v>
+      </c>
+      <c r="J1308" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1308" s="12"/>
+    </row>
+    <row r="1309" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1309" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="B1309" s="1" t="s">
+        <v>4529</v>
+      </c>
+      <c r="C1309" s="1" t="s">
+        <v>4528</v>
+      </c>
+      <c r="D1309" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1309" s="29" t="s">
+        <v>4527</v>
+      </c>
+      <c r="F1309" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1309" s="39" t="s">
+        <v>4526</v>
+      </c>
+      <c r="H1309" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1309" s="1">
+        <v>19059854898</v>
+      </c>
+      <c r="J1309" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1309" s="12"/>
+    </row>
+    <row r="1310" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1310" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1310" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="C1310" s="1" t="s">
+        <v>4532</v>
+      </c>
+      <c r="D1310" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1310" s="29" t="s">
+        <v>4531</v>
+      </c>
+      <c r="F1310" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1310" s="39" t="s">
+        <v>4530</v>
+      </c>
+      <c r="H1310" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1310" s="1">
+        <v>16137661246</v>
+      </c>
+      <c r="J1310" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1310" s="12"/>
+    </row>
+    <row r="1311" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1311" s="1" t="s">
+        <v>2453</v>
+      </c>
+      <c r="B1311" s="1" t="s">
+        <v>4535</v>
+      </c>
+      <c r="C1311" s="1" t="s">
+        <v>4534</v>
+      </c>
+      <c r="D1311" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1311" s="29" t="s">
+        <v>4048</v>
+      </c>
+      <c r="F1311" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1311" s="39" t="s">
+        <v>4533</v>
+      </c>
+      <c r="H1311" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I1311" s="1">
+        <v>16134784848</v>
+      </c>
+      <c r="J1311" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1312" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1312" s="1" t="s">
+        <v>4538</v>
+      </c>
+      <c r="C1312" s="1" t="s">
+        <v>4537</v>
+      </c>
+      <c r="D1312" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1312" s="29" t="s">
+        <v>4536</v>
+      </c>
+      <c r="F1312" s="6" t="s">
+        <v>4108</v>
+      </c>
+      <c r="G1312" s="31"/>
+      <c r="H1312" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1312" s="1">
+        <v>16132708800</v>
+      </c>
+      <c r="J1312" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1313" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1313" s="1" t="s">
+        <v>533</v>
+      </c>
+      <c r="B1313" s="1" t="s">
+        <v>4538</v>
+      </c>
+      <c r="C1313" s="1" t="s">
+        <v>4539</v>
+      </c>
+      <c r="D1313" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1313" s="29" t="s">
+        <v>4536</v>
+      </c>
+      <c r="F1313" s="6" t="s">
+        <v>4108</v>
+      </c>
+      <c r="G1313" s="31"/>
+      <c r="H1313" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1313" s="1">
+        <v>16138341420</v>
+      </c>
+      <c r="J1313" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1314" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1314" s="1" t="s">
+        <v>4538</v>
+      </c>
+      <c r="C1314" s="1" t="s">
+        <v>4540</v>
+      </c>
+      <c r="D1314" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1314" s="29" t="s">
+        <v>4536</v>
+      </c>
+      <c r="F1314" s="6" t="s">
+        <v>4108</v>
+      </c>
+      <c r="G1314" s="31"/>
+      <c r="H1314" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1314" s="1">
+        <v>16137921414</v>
+      </c>
+      <c r="J1314" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1315" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1315" s="1" t="s">
+        <v>4544</v>
+      </c>
+      <c r="C1315" s="1" t="s">
+        <v>4543</v>
+      </c>
+      <c r="D1315" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1315" s="29" t="s">
+        <v>4542</v>
+      </c>
+      <c r="F1315" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1315" s="39" t="s">
+        <v>4541</v>
+      </c>
+      <c r="H1315" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I1315" s="1">
+        <v>15193045040</v>
+      </c>
+      <c r="J1315" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1316" s="1" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B1316" s="1" t="s">
+        <v>1592</v>
+      </c>
+      <c r="C1316" s="1" t="s">
+        <v>4547</v>
+      </c>
+      <c r="D1316" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1316" s="29" t="s">
+        <v>4546</v>
+      </c>
+      <c r="F1316" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1316" s="39" t="s">
+        <v>4545</v>
+      </c>
+      <c r="H1316" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1316" s="1">
+        <v>18072150047</v>
+      </c>
+      <c r="J1316" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1317" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1317" s="1" t="s">
+        <v>4551</v>
+      </c>
+      <c r="C1317" s="1" t="s">
+        <v>4550</v>
+      </c>
+      <c r="D1317" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1317" s="29" t="s">
+        <v>4549</v>
+      </c>
+      <c r="F1317" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1317" s="39"/>
+      <c r="H1317" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1317" s="1">
+        <v>16475378802</v>
+      </c>
+      <c r="J1317" s="1" t="s">
+        <v>4548</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1318" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="B1318" s="1" t="s">
+        <v>4555</v>
+      </c>
+      <c r="C1318" s="1" t="s">
+        <v>4554</v>
+      </c>
+      <c r="D1318" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1318" s="29" t="s">
+        <v>4553</v>
+      </c>
+      <c r="F1318" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1318" s="39" t="s">
+        <v>4552</v>
+      </c>
+      <c r="H1318" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1318" s="1">
+        <v>19057996001</v>
+      </c>
+      <c r="J1318" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1319" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1319" s="1" t="s">
+        <v>4559</v>
+      </c>
+      <c r="C1319" s="1" t="s">
+        <v>4558</v>
+      </c>
+      <c r="D1319" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1319" s="29" t="s">
+        <v>4557</v>
+      </c>
+      <c r="F1319" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1319" s="39" t="s">
+        <v>4556</v>
+      </c>
+      <c r="H1319" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="I1319" s="1">
+        <v>14165198265</v>
+      </c>
+      <c r="J1319" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1320" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1320" s="1" t="s">
+        <v>2795</v>
+      </c>
+      <c r="C1320" s="1" t="s">
+        <v>4561</v>
+      </c>
+      <c r="D1320" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1320" s="29" t="s">
+        <v>4531</v>
+      </c>
+      <c r="F1320" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1320" s="39" t="s">
+        <v>4560</v>
+      </c>
+      <c r="H1320" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1320" s="1">
+        <v>16138294111</v>
+      </c>
+      <c r="J1320" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1321" s="1" t="s">
+        <v>1064</v>
+      </c>
+      <c r="B1321" s="1" t="s">
+        <v>4564</v>
+      </c>
+      <c r="C1321" s="1" t="s">
+        <v>4563</v>
+      </c>
+      <c r="D1321" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1321" s="29" t="s">
+        <v>4562</v>
+      </c>
+      <c r="F1321" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1321" s="31"/>
+      <c r="H1321" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1321" s="1">
+        <v>19055711842</v>
+      </c>
+      <c r="J1321" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1322" s="1" t="s">
+        <v>4568</v>
+      </c>
+      <c r="B1322" s="1" t="s">
+        <v>4567</v>
+      </c>
+      <c r="C1322" s="1" t="s">
+        <v>4566</v>
+      </c>
+      <c r="D1322" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1322" s="29" t="s">
+        <v>4565</v>
+      </c>
+      <c r="F1322" s="6" t="s">
+        <v>1448</v>
+      </c>
+      <c r="G1322" s="31"/>
+      <c r="H1322" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1322" s="1">
+        <v>17053859333</v>
+      </c>
+      <c r="J1322" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:10" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1323" s="1" t="s">
+        <v>2223</v>
+      </c>
+      <c r="B1323" s="1" t="s">
+        <v>4372</v>
+      </c>
+      <c r="C1323" s="1" t="s">
+        <v>2222</v>
+      </c>
+      <c r="D1323" s="11" t="s">
+        <v>4371</v>
+      </c>
+      <c r="E1323" s="33" t="s">
+        <v>1904</v>
+      </c>
+      <c r="F1323" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1323" s="31" t="s">
+        <v>2221</v>
+      </c>
+      <c r="H1323" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="I1323" s="25">
+        <v>16136731313</v>
+      </c>
+      <c r="J1323" s="1" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -56682,9 +57860,10 @@
     <hyperlink ref="E1170" r:id="rId52"/>
     <hyperlink ref="E1181" r:id="rId53"/>
     <hyperlink ref="E1237" r:id="rId54"/>
+    <hyperlink ref="E1307" r:id="rId55"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId55"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId56"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
create buddi delivery scanner and tested
</commit_message>
<xml_diff>
--- a/platform_scrapper/CANNABIS_RESULTS/found_IDs.xlsx
+++ b/platform_scrapper/CANNABIS_RESULTS/found_IDs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14481" uniqueCount="5480">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14489" uniqueCount="5484">
   <si>
     <t>BURLINGTON</t>
   </si>
@@ -16456,13 +16456,25 @@
   </si>
   <si>
     <t>WOW WORLD OF WEED</t>
+  </si>
+  <si>
+    <t>http://41cannabisco.ca/</t>
+  </si>
+  <si>
+    <t>12278 HIGHWAY 41 RR 1</t>
+  </si>
+  <si>
+    <t>41 Cannabis Company</t>
+  </si>
+  <si>
+    <t>NORTHBROOK</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -16574,6 +16586,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -16635,7 +16655,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
@@ -16691,6 +16711,7 @@
     <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Гиперссылка" xfId="2" builtinId="8"/>
@@ -16994,10 +17015,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N1674"/>
+  <dimension ref="A1:N1675"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A1647" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1674" sqref="F1674"/>
+      <selection activeCell="L1649" sqref="L1649"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17007,7 +17028,9 @@
     <col min="5" max="5" width="14.33203125" style="28" customWidth="1"/>
     <col min="6" max="6" width="14.33203125" customWidth="1"/>
     <col min="7" max="7" width="14.33203125" style="24" customWidth="1"/>
-    <col min="8" max="14" width="14.33203125" customWidth="1"/>
+    <col min="8" max="10" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="11.109375" customWidth="1"/>
+    <col min="12" max="14" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
@@ -71571,6 +71594,36 @@
         <v>20</v>
       </c>
       <c r="N1674" s="12"/>
+    </row>
+    <row r="1675" spans="1:14" s="1" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1675" s="1" t="s">
+        <v>5483</v>
+      </c>
+      <c r="B1675" s="1" t="s">
+        <v>5482</v>
+      </c>
+      <c r="C1675" s="1" t="s">
+        <v>5481</v>
+      </c>
+      <c r="D1675" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1675" s="1" t="s">
+        <v>5480</v>
+      </c>
+      <c r="F1675" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="G1675" s="35"/>
+      <c r="H1675" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1675" s="1">
+        <v>16133360441</v>
+      </c>
+      <c r="J1675" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>